<commit_message>
Pending Home Page for 7 Nov
</commit_message>
<xml_diff>
--- a/assets/Mentor Profiles.xlsx
+++ b/assets/Mentor Profiles.xlsx
@@ -106,7 +106,7 @@
     <t>MHA, STB</t>
   </si>
   <si>
-    <t>AI &amp; Machine Learning, User Experience (UX) and User Interface (UI)</t>
+    <t>AI &amp; Machine Learning, User Experience (UX) &amp; User Interface (UI)</t>
   </si>
   <si>
     <t>../assets/img-ng-zhi-hao.jpg</t>
@@ -169,7 +169,7 @@
     <t>Sentosa, MFA</t>
   </si>
   <si>
-    <t>User Experience (UX) and User Interface (UI), Career Development</t>
+    <t>User Experience (UX) &amp; User Interface (UI), Career Development</t>
   </si>
   <si>
     <t>../assets/img-singharvind.jpg</t>
@@ -274,7 +274,7 @@
     <t>A*STAR, Enterprise SG</t>
   </si>
   <si>
-    <t>User Experience (UX) and User Interface (UI), Software Engineering</t>
+    <t>User Experience (UX) &amp; User Interface (UI), Software Engineering</t>
   </si>
   <si>
     <t>../assets/img-zhixuan.jpg</t>
@@ -340,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -359,6 +359,9 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -693,7 +696,7 @@
       <c r="D5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>31</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -765,7 +768,7 @@
       <c r="D8" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>52</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -885,7 +888,7 @@
       <c r="D13" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F13" s="4" t="s">
@@ -920,34 +923,34 @@
       <c r="I22" s="3"/>
     </row>
     <row r="23">
-      <c r="I23" s="7"/>
+      <c r="I23" s="8"/>
     </row>
     <row r="24">
-      <c r="I24" s="7"/>
+      <c r="I24" s="8"/>
     </row>
     <row r="25">
-      <c r="I25" s="7"/>
+      <c r="I25" s="8"/>
     </row>
     <row r="26">
-      <c r="I26" s="7"/>
+      <c r="I26" s="8"/>
     </row>
     <row r="27">
-      <c r="I27" s="7"/>
+      <c r="I27" s="8"/>
     </row>
     <row r="28">
-      <c r="I28" s="7"/>
+      <c r="I28" s="8"/>
     </row>
     <row r="29">
-      <c r="I29" s="7"/>
+      <c r="I29" s="8"/>
     </row>
     <row r="30">
-      <c r="I30" s="7"/>
+      <c r="I30" s="8"/>
     </row>
     <row r="31">
-      <c r="I31" s="7"/>
+      <c r="I31" s="8"/>
     </row>
     <row r="32">
-      <c r="I32" s="7"/>
+      <c r="I32" s="8"/>
     </row>
     <row r="33">
       <c r="I33" s="3"/>

</xml_diff>

<commit_message>
Updated Years of Exp in profile results
</commit_message>
<xml_diff>
--- a/assets/Mentor Profiles.xlsx
+++ b/assets/Mentor Profiles.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
   <si>
     <t>Name</t>
   </si>
@@ -34,6 +34,12 @@
     <t>Email</t>
   </si>
   <si>
+    <t>Years of experience</t>
+  </si>
+  <si>
+    <t>About me</t>
+  </si>
+  <si>
     <t>Joseph Leong</t>
   </si>
   <si>
@@ -55,6 +61,10 @@
     <t>josephleong@mddi.gov.sg</t>
   </si>
   <si>
+    <t>As a President’s Scholarship and Singapore Armed Forces Overseas Scholarship recipient, I have dedicated over 30 years to serving Singapore in both military and civil service roles. Appointed to the Administrative Service in 1995, I ascended through the ranks to Rear-Admiral, holding key leadership positions such as Fleet Commander, Director of Military Intelligence, and Chief of Command during my 24-year military career. 
+Since transitioning to public service in 2019 as Permanent Secretary (Digital Development and Information), I have led the country’s digital transformation efforts, shaping policy and driving initiatives that enhance government services, bolster cybersecurity, and foster the growth of emerging technologies. I also serve as Chairman of the GovTech Board, helping guide the digital agenda for Singapore's future.</t>
+  </si>
+  <si>
     <t>Feng-Ji Sim</t>
   </si>
   <si>
@@ -73,6 +83,10 @@
     <t>fengjisim@mddi.gov.sg</t>
   </si>
   <si>
+    <t>As the Deputy Secretary for Smart Nation and Digital Government, I am privileged to lead Singapore’s digital transformation journey, impacting key areas such as urban living, transport, and government services. My role focuses on making the country’s digital infrastructure more seamless and connected, while advancing the broader vision of a Smart Nation that benefits citizens, businesses, and the economy. 
+Before this, I led the Income Security Policy Division at the Ministry of Manpower, where I focused on financial security and social protection policies. I have also been an active contributor to Singapore's economic planning, having served on both the Committee on the Future Economy and the Economic Strategies Committee.</t>
+  </si>
+  <si>
     <t>Tan Wei Ling</t>
   </si>
   <si>
@@ -94,6 +108,10 @@
     <t>tanweiling@astar.gov.sg</t>
   </si>
   <si>
+    <t>I am the Chief Technology Officer at A*STAR, where I lead the agency’s vision of advancing cutting-edge science and technology in Singapore. Over the course of my career, I have held various roles at IMDA and ICSA, which have deepened my passion for leveraging technology to create solutions that address both business and societal needs.
+My expertise lies in cloud computing, and I am committed to enabling organizations to scale and innovate through secure, agile, and sustainable tech solutions. I am also deeply passionate about mentoring and supporting individuals in their tech career development, guiding the next generation of leaders as they navigate an ever-evolving industry.</t>
+  </si>
+  <si>
     <t>Ng Zhi Hao</t>
   </si>
   <si>
@@ -115,6 +133,10 @@
     <t>ngzhihao@tech.gov.sg</t>
   </si>
   <si>
+    <t>I am a data governance expert and the Head of Data Governance at GovTech, where my primary focus is ensuring that data is securely and effectively managed to support Singapore’s growing digital landscape. I am passionate about leveraging AI, machine learning, and other emerging technologies to drive digital transformation across sectors.
+Throughout my career, I have had the privilege of working with a variety of organizations, including MHA and STB, where I developed expertise in data strategy, analytics, and governance. My goal is to unlock the full potential of data while ensuring privacy, security, and compliance to foster a sustainable digital economy.</t>
+  </si>
+  <si>
     <t>Lee Jia Min</t>
   </si>
   <si>
@@ -136,6 +158,10 @@
     <t>leejiamin@csa.gov.sg</t>
   </si>
   <si>
+    <t>I am the Head of Software Engineering at the Cyber Security Agency of Singapore (CSA), where I lead a talented team of engineers dedicated to developing and deploying cybersecurity solutions to protect Singapore’s critical infrastructure. With over 20 years of experience across various government agencies like MINDEF and SSG, I have honed my skills in software engineering and cybersecurity.
+I’m particularly passionate about the intersection of technology policy management and cybersecurity, where I aim to build resilient systems that not only protect national interests but also foster innovation. Mentoring professionals in tech is something I deeply enjoy, especially guiding them in leadership, career growth, and adapting to the ever-evolving cybersecurity landscape.</t>
+  </si>
+  <si>
     <t>Koh Wei Jie</t>
   </si>
   <si>
@@ -157,6 +183,10 @@
     <t>kohweijie@pmo.gov.sg</t>
   </si>
   <si>
+    <t>I am the Product Architect Lead at the Prime Minister’s Office (PMO), where I design and lead innovative digital solutions that support Singapore’s national strategies. With my extensive background in cloud computing and software engineering, my focus is on building scalable, high-performance products that meet the needs of government stakeholders, enhancing efficiency and productivity.
+Before joining PMO, I worked at GovTech and Sentosa, where I gained valuable experience in solving complex technical challenges and creating impactful solutions. I am deeply passionate about software engineering, cloud computing, and mentoring the next generation of engineers, helping them realize their full potential in the field.</t>
+  </si>
+  <si>
     <t>Singh Arvind</t>
   </si>
   <si>
@@ -178,6 +208,9 @@
     <t>singharvind@jtc.gov.sg</t>
   </si>
   <si>
+    <t>Arvind Singh is an accomplished Chief Innovation Officer at JTC, where he spearheads initiatives to drive digital transformation and innovation. With extensive experience in User Experience (UX) &amp; User Interface (UI) design, Arvind has contributed significantly to enhancing the overall digital experience across various platforms. Prior to his role at JTC, Arvind worked with the Ministry of Foreign Affairs (MFA) and Sentosa Development Corporation, focusing on both innovation and strategic development. With 18 years of experience, he is passionate about shaping the future of user-centric design in the public and private sectors.</t>
+  </si>
+  <si>
     <t>Jonathan Sim</t>
   </si>
   <si>
@@ -199,6 +232,9 @@
     <t>jonsim@htx@gov.sg</t>
   </si>
   <si>
+    <t>Jonathan Sim is the Chief Data Officer at HTX, where he leads the agency's data and artificial intelligence (AI) initiatives, providing strategic direction on emerging technologies. Jonathan has over 19 years of experience in the field of data science, AI, and machine learning, with a background in web development. Having previously worked with the Land Transport Authority (LTA) and the Ministry of Manpower (MOM), Jonathan brings a wealth of knowledge in applying advanced analytics and AI to real-world challenges. He is a firm believer in the potential of data to drive smarter decision-making and sustainable innovations.</t>
+  </si>
+  <si>
     <t>Henry Tiah</t>
   </si>
   <si>
@@ -220,6 +256,9 @@
     <t>gohweiboon@dsta.gov.sg</t>
   </si>
   <si>
+    <t>Henry Tiah is the Head of Digital Transformation at DSTA, where he plays a pivotal role in leading the strategic integration of cutting-edge technologies in defense and security. With over 25 years of experience, Henry has worked across multiple sectors, including the Economic Development Board (EDB) and the Defence Science and Technology Agency (DIS). His expertise in leadership and management, combined with his deep knowledge of tech policy, has made him a highly sought-after mentor in guiding organizations through the complexities of digital transformation.</t>
+  </si>
+  <si>
     <t>Chia Jun Wei</t>
   </si>
   <si>
@@ -241,6 +280,9 @@
     <t>chiajunwei@psd.gov.sg</t>
   </si>
   <si>
+    <t>Chia Jun Wei is a Senior Director for Cloud Infrastructure at the Public Service Division (PSD), where he leads cloud adoption strategies and ensures the seamless integration of cloud technologies across various government agencies. With a background in Cloud Computing and 11 years of industry experience, Jun Wei has played an instrumental role in enhancing the government’s digital infrastructure. His leadership in both technical execution and strategic management has contributed to the successful deployment of cloud solutions at the Singapore Land Authority (SLA) and Ministry of Education (MOE).</t>
+  </si>
+  <si>
     <t>Tan Su Ling</t>
   </si>
   <si>
@@ -262,6 +304,10 @@
     <t>tansuling@imda.gov.sg</t>
   </si>
   <si>
+    <t xml:space="preserve">Tan Su Ling is a Senior Vice President of Engineering at the Infocomm Media Development Authority (IMDA), where she leads high-impact engineering teams dedicated to developing innovative solutions for the digital economy. With 10 years of experience in software engineering and career development, Su Ling has been a driving force behind the successful rollout of several digital initiatives at Synapxe and Civil Aviation Authority of Singapore (CAAS). She is passionate about mentoring the next generation of engineers and empowering them with the skills necessary to thrive in an evolving tech landscape.
+</t>
+  </si>
+  <si>
     <t>Liu Zhi Xuan</t>
   </si>
   <si>
@@ -281,6 +327,9 @@
   </si>
   <si>
     <t>liuzhixuan@nrf.gov.sg</t>
+  </si>
+  <si>
+    <t>Liu Zhi Xuan is the Director of Digital Innovation at the National Research Foundation (NRF), where he leads efforts to harness digital technologies to push forward Singapore’s innovation agenda. With 12 years of experience in both Software Engineering and User Experience (UX) &amp; User Interface (UI) design, Zhi Xuan has worked extensively with A*STAR and Enterprise Singapore to shape the country’s digital future. Zhi Xuan is passionate about developing user-centered digital products and ensuring that new technologies are aligned with user needs for maximum impact.</t>
   </si>
 </sst>
 </file>
@@ -301,11 +350,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="FF800000"/>
-      <name val="Consolas"/>
-    </font>
-    <font>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -313,6 +357,11 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF800000"/>
+      <name val="Consolas"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -340,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -350,18 +399,21 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -585,6 +637,7 @@
     <col customWidth="1" min="2" max="2" width="45.25"/>
     <col customWidth="1" min="4" max="4" width="42.25"/>
     <col customWidth="1" min="5" max="5" width="73.13"/>
+    <col customWidth="1" min="9" max="9" width="85.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -609,390 +662,456 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3"/>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="3">
+        <v>30.0</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="3">
+        <v>21.0</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>21</v>
+      <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="3">
+        <v>18.0</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>29</v>
+      <c r="A5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="3">
+        <v>17.0</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>36</v>
+      <c r="A6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>42</v>
+      <c r="A7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I7" s="3"/>
+        <v>52</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="3">
+        <v>19.0</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>49</v>
+      <c r="A8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8" s="3"/>
+        <v>59</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="3">
+        <v>18.0</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>57</v>
+      <c r="A9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="3"/>
+        <v>68</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="3">
+        <v>19.0</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>64</v>
+      <c r="A10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I10" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="3">
+        <v>25.0</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>70</v>
+      <c r="A11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="I11" s="3"/>
+        <v>84</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H11" s="3">
+        <v>11.0</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>78</v>
+      <c r="A12" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="I12" s="3"/>
+        <v>92</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H12" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>88</v>
+        <v>100</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>89</v>
+        <v>102</v>
+      </c>
+      <c r="H13" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="15">
-      <c r="I15" s="3"/>
+      <c r="I15" s="8"/>
     </row>
     <row r="16">
-      <c r="I16" s="3"/>
+      <c r="I16" s="8"/>
     </row>
     <row r="17">
-      <c r="I17" s="3"/>
+      <c r="I17" s="8"/>
     </row>
     <row r="18">
-      <c r="I18" s="3"/>
+      <c r="I18" s="8"/>
     </row>
     <row r="19">
-      <c r="I19" s="3"/>
+      <c r="I19" s="8"/>
     </row>
     <row r="20">
-      <c r="I20" s="3"/>
+      <c r="I20" s="8"/>
     </row>
     <row r="21">
-      <c r="I21" s="3"/>
+      <c r="I21" s="8"/>
     </row>
     <row r="22">
-      <c r="I22" s="3"/>
+      <c r="I22" s="8"/>
     </row>
     <row r="23">
-      <c r="I23" s="8"/>
+      <c r="I23" s="9"/>
     </row>
     <row r="24">
-      <c r="I24" s="8"/>
+      <c r="I24" s="9"/>
     </row>
     <row r="25">
-      <c r="I25" s="8"/>
+      <c r="I25" s="9"/>
     </row>
     <row r="26">
-      <c r="I26" s="8"/>
+      <c r="I26" s="9"/>
     </row>
     <row r="27">
-      <c r="I27" s="8"/>
+      <c r="I27" s="9"/>
     </row>
     <row r="28">
-      <c r="I28" s="8"/>
+      <c r="I28" s="9"/>
     </row>
     <row r="29">
-      <c r="I29" s="8"/>
+      <c r="I29" s="9"/>
     </row>
     <row r="30">
-      <c r="I30" s="8"/>
+      <c r="I30" s="9"/>
     </row>
     <row r="31">
-      <c r="I31" s="8"/>
+      <c r="I31" s="9"/>
     </row>
     <row r="32">
-      <c r="I32" s="8"/>
+      <c r="I32" s="9"/>
     </row>
     <row r="33">
-      <c r="I33" s="3"/>
+      <c r="I33" s="8"/>
     </row>
     <row r="34">
-      <c r="I34" s="3"/>
+      <c r="I34" s="8"/>
     </row>
     <row r="35">
-      <c r="I35" s="3"/>
+      <c r="I35" s="8"/>
     </row>
     <row r="36">
-      <c r="I36" s="3"/>
+      <c r="I36" s="8"/>
     </row>
     <row r="37">
-      <c r="I37" s="3"/>
+      <c r="I37" s="8"/>
     </row>
     <row r="38">
-      <c r="I38" s="3"/>
+      <c r="I38" s="8"/>
     </row>
     <row r="39">
-      <c r="I39" s="3"/>
+      <c r="I39" s="8"/>
     </row>
     <row r="40">
-      <c r="I40" s="3"/>
+      <c r="I40" s="8"/>
     </row>
     <row r="41">
-      <c r="I41" s="3"/>
+      <c r="I41" s="8"/>
     </row>
     <row r="42">
-      <c r="I42" s="3"/>
+      <c r="I42" s="8"/>
     </row>
     <row r="43">
-      <c r="I43" s="3"/>
+      <c r="I43" s="8"/>
     </row>
     <row r="44">
-      <c r="I44" s="3"/>
+      <c r="I44" s="8"/>
     </row>
     <row r="45">
-      <c r="I45" s="3"/>
+      <c r="I45" s="8"/>
     </row>
     <row r="46">
-      <c r="I46" s="3"/>
+      <c r="I46" s="8"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
More Profiles Added v1
</commit_message>
<xml_diff>
--- a/assets/Mentor Profiles.xlsx
+++ b/assets/Mentor Profiles.xlsx
@@ -5,13 +5,15 @@
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$M$2:$N$49</definedName>
+  </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="246">
   <si>
     <t>Name</t>
   </si>
@@ -330,6 +332,432 @@
   </si>
   <si>
     <t>Liu Zhi Xuan is the Director of Digital Innovation at the National Research Foundation (NRF), where he leads efforts to harness digital technologies to push forward Singapore’s innovation agenda. With 12 years of experience in both Software Engineering and User Experience (UX) &amp; User Interface (UI) design, Zhi Xuan has worked extensively with A*STAR and Enterprise Singapore to shape the country’s digital future. Zhi Xuan is passionate about developing user-centered digital products and ensuring that new technologies are aligned with user needs for maximum impact.</t>
+  </si>
+  <si>
+    <t>Wong Rui En</t>
+  </si>
+  <si>
+    <t>Chief Information Officer (CIO)</t>
+  </si>
+  <si>
+    <t>SLA, HDB</t>
+  </si>
+  <si>
+    <t>Web Development, Leadership and Management, Tech Policy Management</t>
+  </si>
+  <si>
+    <t>../assets/img-ruien.jpg</t>
+  </si>
+  <si>
+    <t>wongruien@imda.gov.sg</t>
+  </si>
+  <si>
+    <t>Wong Rui En is the Chief Information Officer (CIO) at the Infocomm Media Development Authority (IMDA). With over 15 years of experience in Web Development, Leadership, and Tech Policy Management, Rui En has worked across various sectors, including the Singapore Land Authority (SLA) and the Housing &amp; Development Board (HDB). She is deeply involved in shaping Singapore's digital transformation, focusing on integrating innovative technologies and ensuring effective governance of digital platforms. Rui En is passionate about driving organizational change through technology and creating sustainable digital solutions for public services.</t>
+  </si>
+  <si>
+    <t>Chong Mei Ying</t>
+  </si>
+  <si>
+    <t>Head of Artificial Intelligence (AI) Engineering</t>
+  </si>
+  <si>
+    <t>LTA</t>
+  </si>
+  <si>
+    <t>NLB, MINDEF</t>
+  </si>
+  <si>
+    <t>AI &amp; Machine Learning, Software Engineering, Web Development</t>
+  </si>
+  <si>
+    <t>../assets/img-meiying.jpg</t>
+  </si>
+  <si>
+    <t>chongmeiying@lta.gov.sg</t>
+  </si>
+  <si>
+    <t>Chong Mei Ying is the Head of Artificial Intelligence (AI) Engineering at the Land Transport Authority (LTA), where she leads the AI strategy and engineering efforts to enhance Singapore’s transport systems. With 18 years of experience in AI &amp; Machine Learning, Software Engineering, and Web Development, Mei Ying has previously contributed to key projects at the National Library Board (NLB) and the Ministry of Defence (MINDEF). She is an advocate for the transformative power of AI in smart cities, focusing on innovative solutions that can improve public services and urban mobility.</t>
+  </si>
+  <si>
+    <t>Lim Yuhang</t>
+  </si>
+  <si>
+    <t>Director of Machine Learning Operations (MLOps)</t>
+  </si>
+  <si>
+    <t>CPFB, Enterprise SG</t>
+  </si>
+  <si>
+    <t>Cloud Computing, AI &amp; Machine Learning, Career Development</t>
+  </si>
+  <si>
+    <t>../assets/img-yuhang.jpg</t>
+  </si>
+  <si>
+    <t>limyuhang@htx.gov.sg</t>
+  </si>
+  <si>
+    <t>Lim Yuhang is the Director of Machine Learning Operations (MLOps) at HTX, where he drives the integration of machine learning models into real-world applications for various government agencies. With 17 years of experience in Cloud Computing, AI &amp; Machine Learning, and Career Development, Yuhang has worked with agencies such as CPFB and Enterprise Singapore. He is committed to advancing Singapore’s AI capabilities, particularly in operationalizing machine learning models, and is passionate about mentoring the next generation of AI talent in Singapore’s public sector.</t>
+  </si>
+  <si>
+    <t>Goh Jie Wei</t>
+  </si>
+  <si>
+    <t>Head of Cybersecurity Strategy</t>
+  </si>
+  <si>
+    <t>A*STAR, SLA, NLB</t>
+  </si>
+  <si>
+    <t>Tech Policy Management, Cybersecurity</t>
+  </si>
+  <si>
+    <t>../assets/img-jiewei.jpg</t>
+  </si>
+  <si>
+    <t>gohjiewei@csa.gov.sg</t>
+  </si>
+  <si>
+    <t>Goh Jie Wei is the Head of Cybersecurity Strategy at the Cyber Security Agency of Singapore (CSA). With over 25 years of experience in Cybersecurity and Tech Policy Management, Jie Wei has held leadership positions at organizations like A*STAR and the Singapore Land Authority (SLA). He plays a critical role in shaping Singapore’s national cybersecurity strategy and policies. Jie Wei is dedicated to enhancing the nation’s digital resilience and ensuring that cybersecurity becomes an integral part of every technological innovation.</t>
+  </si>
+  <si>
+    <t>Chua Tian Wei</t>
+  </si>
+  <si>
+    <t>Senior Director of Cloud Solutions</t>
+  </si>
+  <si>
+    <t>IRAS</t>
+  </si>
+  <si>
+    <t>GovTech, MOH</t>
+  </si>
+  <si>
+    <t>Career Development, Data Science &amp; Analytics, Cloud Computing</t>
+  </si>
+  <si>
+    <t>../assets/img-tianwei.jpg</t>
+  </si>
+  <si>
+    <t>chuatianwei@iras.gov.sg</t>
+  </si>
+  <si>
+    <t>Chua Tian Wei is the Senior Director of Cloud Solutions at the Inland Revenue Authority of Singapore (IRAS). With 20 years of experience spanning Data Science &amp; Analytics, Cloud Computing, and Career Development, Tian Wei has been instrumental in driving cloud adoption at key government agencies such as GovTech and the Ministry of Health (MOH). His expertise lies in developing scalable cloud strategies that enable seamless digital government services, and he is passionate about empowering teams to thrive in cloud-first environments.</t>
+  </si>
+  <si>
+    <t>Tan Ming Wei</t>
+  </si>
+  <si>
+    <t>Director of Product Development</t>
+  </si>
+  <si>
+    <t>MFA</t>
+  </si>
+  <si>
+    <t>MCCY, CSC, SSG</t>
+  </si>
+  <si>
+    <t>User Experience (UX) &amp; User Interface (UI), Web Development, Tech Policy Management, Mobile App Development</t>
+  </si>
+  <si>
+    <t>../assets/img-mingwei.jpg</t>
+  </si>
+  <si>
+    <t>tanminghui@mfa.gov.sg</t>
+  </si>
+  <si>
+    <t>Tan Ming Hui is the Director of Product Development at the Ministry of Foreign Affairs (MFA), where she oversees the development of digital products and solutions that enhance user experiences and engagement. With over 23 years of experience in User Experience (UX) &amp; User Interface (UI), Web Development, and Mobile App Development, Ming Hui has worked across various sectors, including the Ministry of Culture, Community, and Youth (MCCY) and the Civil Service College (CSC). She is committed to creating intuitive, user-centered digital products that bridge the gap between technology and public service.</t>
+  </si>
+  <si>
+    <t>Ng Jia Yuan</t>
+  </si>
+  <si>
+    <t>Head of Blockchain Innovation</t>
+  </si>
+  <si>
+    <t>MOF</t>
+  </si>
+  <si>
+    <t>MSF, MSE, PUB</t>
+  </si>
+  <si>
+    <t>Tech Policy Management, AI &amp; Machine Learning, Software Engineering</t>
+  </si>
+  <si>
+    <t>../assets/img-jiayuan.jpg</t>
+  </si>
+  <si>
+    <t>ngjiayuan@mof.gov.sg</t>
+  </si>
+  <si>
+    <t>Ng Jia Yuan is the Head of Blockchain Innovation at the Ministry of Finance (MOF). With 22 years of experience in AI &amp; Machine Learning, Software Engineering, and Tech Policy Management, Jia Yuan has previously worked with the Ministry of Social and Family Development (MSF) and the Ministry of Trade and Industry (MSE). He leads blockchain initiatives that aim to strengthen Singapore’s position as a global leader in digital finance and fintech. Jia Yuan is passionate about exploring new blockchain use cases to transform government operations and enhance public trust in digital systems.</t>
+  </si>
+  <si>
+    <t>Liu Kai Xuan</t>
+  </si>
+  <si>
+    <t>Senior Data Scientist</t>
+  </si>
+  <si>
+    <t>Enterprise SG</t>
+  </si>
+  <si>
+    <t>A*STAR, GovTech, URA</t>
+  </si>
+  <si>
+    <t>Leadership and Management, Data Science &amp; Analytics</t>
+  </si>
+  <si>
+    <t>../assets/img-kaixuan.jpg</t>
+  </si>
+  <si>
+    <t>liukaixin@esg.gov.sg</t>
+  </si>
+  <si>
+    <t>Liu Kai Xin is a Senior Data Scientist at Enterprise Singapore, where he leads data analytics initiatives to drive business growth and innovation. With 26 years of experience in Leadership and Management and Data Science &amp; Analytics, Kai Xin has also contributed to projects at GovTech and the Urban Redevelopment Authority (URA). He is focused on leveraging data-driven insights to optimize business strategies and foster data-centric innovation within the public sector.</t>
+  </si>
+  <si>
+    <t>Sim Ying Jie</t>
+  </si>
+  <si>
+    <t>Director of Software Quality Assurance</t>
+  </si>
+  <si>
+    <t>MAS</t>
+  </si>
+  <si>
+    <t>GovTech, A*STAR</t>
+  </si>
+  <si>
+    <t>Tech Policy Management, Web Development, Software Engineering</t>
+  </si>
+  <si>
+    <t>../assets/img-yingjie.jpg</t>
+  </si>
+  <si>
+    <t>simyingjie@mas.gov.sg</t>
+  </si>
+  <si>
+    <t>Sim Ying Jie is the Director of Software Quality Assurance at the Monetary Authority of Singapore (MAS). With 14 years of experience in Software Engineering, Web Development, and Tech Policy Management, Ying Jie has worked across several government agencies, including GovTech and A*STAR. He specializes in ensuring the quality and security of digital solutions, advocating for best practices in software development and testing to ensure robust, scalable solutions for financial institutions.</t>
+  </si>
+  <si>
+    <t>Zhang Xuan Wen</t>
+  </si>
+  <si>
+    <t>Chief Digital Officer</t>
+  </si>
+  <si>
+    <t>SSG, URA</t>
+  </si>
+  <si>
+    <t>Tech Policy Management, Leadership and Management, Data Science &amp; Analytics</t>
+  </si>
+  <si>
+    <t>../assets/img-xuanwen.jpg</t>
+  </si>
+  <si>
+    <t>zhangxuanwen@psd.gov.sg</t>
+  </si>
+  <si>
+    <t>Zhang Xuan Wen is the Chief Digital Officer at the Public Service Division (PSD), where he drives digital transformation initiatives to improve government services. With 17 years of experience in Tech Policy Management, Leadership, and Data Science &amp; Analytics, Xuan Wen has previously contributed to significant digital government projects at the Singapore Skills Development Council (SSG) and the Urban Redevelopment Authority (URA). He is passionate about harnessing technology to enable a smarter, more efficient government that can better serve citizens.</t>
+  </si>
+  <si>
+    <t>Lee Wei Kiat</t>
+  </si>
+  <si>
+    <t>Senior Director of AI &amp; Automation</t>
+  </si>
+  <si>
+    <t>MCCY, CSA</t>
+  </si>
+  <si>
+    <t>Web Development, AI &amp; Machine Learning, Career Development</t>
+  </si>
+  <si>
+    <t>../assets/img-weikiat.jpg</t>
+  </si>
+  <si>
+    <t>leewkiat@tech.gov.sg</t>
+  </si>
+  <si>
+    <t>Lee Wei Kiat is the Senior Director of AI &amp; Automation at GovTech, where he leads AI-driven automation projects to optimize government operations. With 13 years of experience in Web Development, AI &amp; Machine Learning, and Career Development, Wei Kiat has previously worked at the Ministry of Culture, Community, and Youth (MCCY) and the Cyber Security Agency (CSA). He is deeply interested in exploring how AI can transform public service delivery and improve citizen experiences.</t>
+  </si>
+  <si>
+    <t>Teo Hui En</t>
+  </si>
+  <si>
+    <t>Head of IT Infrastructure and Operations</t>
+  </si>
+  <si>
+    <t>HDB</t>
+  </si>
+  <si>
+    <t>MOM, Sentosa</t>
+  </si>
+  <si>
+    <t>Cloud Computing, AI &amp; Machine Learning</t>
+  </si>
+  <si>
+    <t>../assets/img-huien.jpg</t>
+  </si>
+  <si>
+    <t>teohui.en@hdb.gov.sg</t>
+  </si>
+  <si>
+    <t>Teo Hui En is the Head of IT Infrastructure and Operations at the Housing &amp; Development Board (HDB), where she oversees the infrastructure that powers HDB’s digital services. With 16 years of experience in Cloud Computing, AI &amp; Machine Learning, and IT Operations, Hui En has worked at MOM and Sentosa Development Corporation, where she led initiatives to modernize IT infrastructure and integrate AI capabilities. She is passionate about creating resilient and scalable infrastructure that can support the government’s digital transformation efforts.</t>
+  </si>
+  <si>
+    <t>Ong Wei Jin</t>
+  </si>
+  <si>
+    <t>Director of UX/UI Design</t>
+  </si>
+  <si>
+    <t>JTC, MSF, CAAS</t>
+  </si>
+  <si>
+    <t>User Experience (UX) &amp; User Interface (UI), Leadership and Management, Career Development</t>
+  </si>
+  <si>
+    <t>../assets/img-weijin.jpg</t>
+  </si>
+  <si>
+    <t>ongweijin@imda.gov.sg</t>
+  </si>
+  <si>
+    <t>Ong Wei Jin is the Director of UX/UI Design at IMDA, where he designs user-centric digital experiences that enhance public service delivery. With 11 years of experience in User Experience (UX) &amp; User Interface (UI), Leadership and Management, and Career Development, Wei Jin has contributed to projects for JTC, MSF, and CAAS. He is passionate about designing inclusive, intuitive interfaces that empower users and improve interactions with government services.</t>
+  </si>
+  <si>
+    <t>Ho Rui Liang</t>
+  </si>
+  <si>
+    <t>Head of Data Science and Analytics</t>
+  </si>
+  <si>
+    <t>Sentosa, STB, MOE</t>
+  </si>
+  <si>
+    <t>../assets/img-ruiliang.jpg</t>
+  </si>
+  <si>
+    <t>horuiliang@tech.gov.sg</t>
+  </si>
+  <si>
+    <t>Ho Rui Liang is the Head of Data Science and Analytics at GovTech, where he leads initiatives to harness the power of data to drive innovation in government services. With 16 years of experience in Leadership and Management and Data Science &amp; Analytics, Rui Liang has previously worked at Sentosa, the Singapore Tourism Board (STB), and the Ministry of Education (MOE). He is committed to driving data-driven decisions to improve public policy and optimize government service delivery.</t>
+  </si>
+  <si>
+    <t>Tan Wei Xuan</t>
+  </si>
+  <si>
+    <t>Senior Director of DevOps Engineering</t>
+  </si>
+  <si>
+    <t>CAAS, MCCY</t>
+  </si>
+  <si>
+    <t>Tech Policy Management, Career Development, Software Engineering</t>
+  </si>
+  <si>
+    <t>../assets/img-weixuan.jpg</t>
+  </si>
+  <si>
+    <t>tanweixuan@tech.gov.sg</t>
+  </si>
+  <si>
+    <t>Tan Wei Xuan is the Senior Director of DevOps Engineering at GovTech, where he leads DevOps initiatives to streamline software development and improve deployment processes. With 15 years of experience in Tech Policy Management, Software Engineering, and Career Development, Wei Xuan has worked at CAAS and MCCY. He is passionate about creating efficient and agile workflows to enable faster and more reliable government service delivery.</t>
+  </si>
+  <si>
+    <t>Chong Zhen Xiong</t>
+  </si>
+  <si>
+    <t>Director of IT Governance &amp; Compliance</t>
+  </si>
+  <si>
+    <t>CSIT</t>
+  </si>
+  <si>
+    <t>LTA, PUB</t>
+  </si>
+  <si>
+    <t>Leadership and Management, Tech Policy Management, Career Development</t>
+  </si>
+  <si>
+    <t>../assets/img-zhenxiong.jpg</t>
+  </si>
+  <si>
+    <t>chongzhenxiong@csit.gov.sg</t>
+  </si>
+  <si>
+    <t>Chong Zhen Xiong is the Director of IT Governance &amp; Compliance at CSIT, where he ensures that the IT systems supporting Singapore’s public sector adhere to rigorous governance standards. With 14 years of experience in Tech Policy Management, Career Development, and Leadership, Zhen Xiong has also worked at LTA and PUB. He is dedicated to ensuring that IT governance frameworks are robust, transparent, and aligned with Singapore’s digital policies.</t>
+  </si>
+  <si>
+    <t>Siva Rajan</t>
+  </si>
+  <si>
+    <t>Head of IT Strategy and Architecture</t>
+  </si>
+  <si>
+    <t>MTI</t>
+  </si>
+  <si>
+    <t>Sentosa, MOT, MAS</t>
+  </si>
+  <si>
+    <t>Software Engineering, Leadership and Management, Career Development</t>
+  </si>
+  <si>
+    <t>../assets/img-sivarajan.jpg</t>
+  </si>
+  <si>
+    <t>sivarajan@mti.gov.sg</t>
+  </si>
+  <si>
+    <t>Siva Rajan is the Head of IT Strategy and Architecture at the Ministry of Trade and Industry (MTI), where he shapes the IT architecture strategy for Singapore’s economic growth. With over 27 years of experience in Software Engineering, Leadership and Management, and Career Development, Siva has previously worked with Sentosa, MOT, and MAS. He is an advocate for strategic IT alignment, focusing on how technology can drive business innovation and economic prosperity.</t>
+  </si>
+  <si>
+    <t>Lim Zi Xuan</t>
+  </si>
+  <si>
+    <t>Director of Smart Cities and IoT</t>
+  </si>
+  <si>
+    <t>CPFB, SLA, MND</t>
+  </si>
+  <si>
+    <t>User Experience (UX) &amp; User Interface (UI), Career Development, Tech Policy Management, Leadership and Management</t>
+  </si>
+  <si>
+    <t>../assets/img-zixuan.jpg</t>
+  </si>
+  <si>
+    <t>limzixuan@mddi.gov.sg</t>
+  </si>
+  <si>
+    <t>Lim Zi Xuan is the Director of Smart Cities and IoT at MDDI (SNDGO), where he leads efforts to build smart, connected cities through IoT solutions. With 29 years of experience in User Experience (UX) &amp; User Interface (UI), Leadership and Management, and Tech Policy Management, Zi Xuan has contributed to projects at CPFB, SLA, and MND. He is passionate about using IoT to enhance urban living, promote sustainability, and improve the quality of life for Singaporeans.</t>
+  </si>
+  <si>
+    <t>Koh Jie Lin</t>
+  </si>
+  <si>
+    <t>Senior Manager, Cloud Architecture and Security</t>
+  </si>
+  <si>
+    <t>EDB</t>
+  </si>
+  <si>
+    <t>SUPCOURT, HTX</t>
+  </si>
+  <si>
+    <t>Cloud Computing, Leadership and Management, Software Engineering</t>
+  </si>
+  <si>
+    <t>../assets/img-jielin.jpg</t>
+  </si>
+  <si>
+    <t>kohjielin@edb.gov.sg</t>
+  </si>
+  <si>
+    <t>Koh Jie Lin is the Senior Manager of Cloud Architecture and Security at the Economic Development Board (EDB), where she leads the design and implementation of cloud security strategies. With 17 years of experience in Cloud Computing, Software Engineering, and Leadership, Jie Lin has worked with the Supreme Court (SUPCOURT) and HTX to develop secure, scalable cloud architectures for public sector applications. She is committed to driving cloud security best practices that protect critical government data while enabling innovation.</t>
   </si>
 </sst>
 </file>
@@ -350,6 +778,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11.0"/>
+      <color rgb="FF800000"/>
+      <name val="Consolas"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -357,11 +790,6 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FF800000"/>
-      <name val="Consolas"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -389,7 +817,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -399,25 +827,24 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -635,7 +1062,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="45.25"/>
-    <col customWidth="1" min="4" max="4" width="42.25"/>
+    <col customWidth="1" min="4" max="4" width="18.5"/>
     <col customWidth="1" min="5" max="5" width="73.13"/>
     <col customWidth="1" min="9" max="9" width="85.75"/>
   </cols>
@@ -668,452 +1095,925 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="2"/>
+      <c r="Q1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="4">
         <v>30.0</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="P2" s="1"/>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="4">
         <v>21.0</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="4">
         <v>18.0</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="4">
         <v>17.0</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="4">
         <v>20.0</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="5" t="s">
         <v>47</v>
       </c>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="3"/>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="4">
         <v>19.0</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="5" t="s">
         <v>55</v>
       </c>
+      <c r="Q7" s="3"/>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="4">
         <v>18.0</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="5" t="s">
         <v>63</v>
       </c>
+      <c r="Q8" s="3"/>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="4">
         <v>19.0</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="5" t="s">
         <v>71</v>
       </c>
+      <c r="Q9" s="3"/>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="4">
         <v>25.0</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="5" t="s">
         <v>79</v>
       </c>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="3"/>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="4">
         <v>11.0</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="5" t="s">
         <v>87</v>
       </c>
+      <c r="Q11" s="3"/>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="4">
         <v>10.0</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="5" t="s">
         <v>95</v>
       </c>
+      <c r="Q12" s="3"/>
     </row>
     <row r="13">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="4">
         <v>12.0</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="5" t="s">
         <v>103</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14" s="4">
+        <v>15.0</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
     <row r="15">
-      <c r="I15" s="8"/>
+      <c r="A15" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15" s="4">
+        <v>18.0</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="16">
-      <c r="I16" s="8"/>
+      <c r="A16" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="H16" s="4">
+        <v>17.0</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="17">
-      <c r="I17" s="8"/>
+      <c r="A17" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="H17" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="18">
-      <c r="I18" s="8"/>
+      <c r="A18" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="H18" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="19">
-      <c r="I19" s="8"/>
+      <c r="A19" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H19" s="4">
+        <v>23.0</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="20">
-      <c r="I20" s="8"/>
+      <c r="A20" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="H20" s="4">
+        <v>22.0</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="21">
-      <c r="I21" s="8"/>
+      <c r="A21" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="H21" s="4">
+        <v>26.0</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="22">
-      <c r="I22" s="8"/>
+      <c r="A22" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="H22" s="4">
+        <v>14.0</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="23">
-      <c r="I23" s="9"/>
+      <c r="A23" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="H23" s="4">
+        <v>17.0</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="24">
-      <c r="I24" s="9"/>
+      <c r="A24" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="H24" s="4">
+        <v>13.0</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="25">
-      <c r="I25" s="9"/>
+      <c r="A25" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="H25" s="4">
+        <v>16.0</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="26">
-      <c r="I26" s="9"/>
+      <c r="A26" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="H26" s="4">
+        <v>11.0</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="27">
-      <c r="I27" s="9"/>
+      <c r="A27" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="H27" s="4">
+        <v>16.0</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="28">
-      <c r="I28" s="9"/>
+      <c r="A28" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="H28" s="4">
+        <v>15.0</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="29">
-      <c r="I29" s="9"/>
+      <c r="A29" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="H29" s="4">
+        <v>14.0</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="30">
-      <c r="I30" s="9"/>
+      <c r="A30" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="H30" s="4">
+        <v>27.0</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="31">
-      <c r="I31" s="9"/>
+      <c r="A31" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="H31" s="4">
+        <v>29.0</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="32">
-      <c r="I32" s="9"/>
-    </row>
-    <row r="33">
-      <c r="I33" s="8"/>
+      <c r="A32" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="H32" s="4">
+        <v>17.0</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="34">
-      <c r="I34" s="8"/>
-    </row>
-    <row r="35">
-      <c r="I35" s="8"/>
-    </row>
-    <row r="36">
-      <c r="I36" s="8"/>
-    </row>
-    <row r="37">
-      <c r="I37" s="8"/>
-    </row>
-    <row r="38">
-      <c r="I38" s="8"/>
-    </row>
-    <row r="39">
-      <c r="I39" s="8"/>
-    </row>
-    <row r="40">
-      <c r="I40" s="8"/>
-    </row>
-    <row r="41">
-      <c r="I41" s="8"/>
-    </row>
-    <row r="42">
-      <c r="I42" s="8"/>
-    </row>
-    <row r="43">
-      <c r="I43" s="8"/>
-    </row>
-    <row r="44">
-      <c r="I44" s="8"/>
-    </row>
-    <row r="45">
-      <c r="I45" s="8"/>
-    </row>
-    <row r="46">
-      <c r="I46" s="8"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="$M$2:$N$49"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pending Agency Filter look and feel
</commit_message>
<xml_diff>
--- a/assets/Mentor Profiles.xlsx
+++ b/assets/Mentor Profiles.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="247">
   <si>
     <t>Name</t>
   </si>
@@ -48,7 +48,7 @@
     <t>Permanent Secretary (Digital Development and Information)</t>
   </si>
   <si>
-    <t>MDDI (SNDGO）</t>
+    <t>MDDI (SNDGO)</t>
   </si>
   <si>
     <t>MINDEF</t>
@@ -719,6 +719,9 @@
   </si>
   <si>
     <t>Director of Smart Cities and IoT</t>
+  </si>
+  <si>
+    <t>MDDI (SNDGO）</t>
   </si>
   <si>
     <t>CPFB, SLA, MND</t>
@@ -1957,54 +1960,54 @@
         <v>232</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>11</v>
+        <v>233</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H31" s="4">
         <v>29.0</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="H32" s="4">
         <v>17.0</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="34">

</xml_diff>

<commit_message>
Final version (pending Agency Filter update)
</commit_message>
<xml_diff>
--- a/assets/Mentor Profiles.xlsx
+++ b/assets/Mentor Profiles.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="246">
   <si>
     <t>Name</t>
   </si>
@@ -719,9 +719,6 @@
   </si>
   <si>
     <t>Director of Smart Cities and IoT</t>
-  </si>
-  <si>
-    <t>MDDI (SNDGO）</t>
   </si>
   <si>
     <t>CPFB, SLA, MND</t>
@@ -1960,54 +1957,54 @@
         <v>232</v>
       </c>
       <c r="C31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="E31" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="F31" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="G31" s="4" t="s">
         <v>236</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>237</v>
       </c>
       <c r="H31" s="4">
         <v>29.0</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="D32" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="F32" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="G32" s="4" t="s">
         <v>244</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>245</v>
       </c>
       <c r="H32" s="4">
         <v>17.0</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34">

</xml_diff>